<commit_message>
framework setup with config, excel, report
</commit_message>
<xml_diff>
--- a/test-data/myapplication-test-data.xlsx
+++ b/test-data/myapplication-test-data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\InteliJ_Project\MavenSelenium\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199A1532-69BA-4E81-B6DB-A98DC8C9306A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A035196D-AFAC-441C-8E19-E70A9AA7DC7B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -42,7 +42,7 @@
     <t>abc@abc.com</t>
   </si>
   <si>
-    <t>xy@abc.com</t>
+    <t>xyz@abc.com</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>